<commit_message>
Started Full NEA document
</commit_message>
<xml_diff>
--- a/Feedback.xlsx
+++ b/Feedback.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93313CF2-48C4-4FF6-9FB3-B9050EFDD889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67C0095-2F5C-4D25-A784-1C5A9E0E4932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Build Version</t>
   </si>
@@ -83,6 +83,14 @@
 - Normal chess AI sometimes freezes
 - Sometimes players appear twice in lobbies
 - AI sometimes doesn't pick best move</t>
+  </si>
+  <si>
+    <t>V1.34</t>
+  </si>
+  <si>
+    <t>- No colour sheme / boring colours
+- No dividers between buttons
+- Make errors display in a nicer way</t>
   </si>
 </sst>
 </file>
@@ -406,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -475,6 +483,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>